<commit_message>
Corrected user survey confusion between pattern and sliding autonomy.
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/DataMyAnalysis.xlsx
+++ b/PathPlanner/UserStudyData/DataMyAnalysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1930,12 +1930,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cone"/>
-        <c:axId val="126925824"/>
-        <c:axId val="110945984"/>
-        <c:axId val="126568320"/>
+        <c:axId val="539103744"/>
+        <c:axId val="538789568"/>
+        <c:axId val="539078656"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="126925824"/>
+        <c:axId val="539103744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,7 +1988,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110945984"/>
+        <c:crossAx val="538789568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1996,7 +1996,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110945984"/>
+        <c:axId val="538789568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,12 +2007,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126925824"/>
+        <c:crossAx val="539103744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="126568320"/>
+        <c:axId val="539078656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2057,7 +2057,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="110945984"/>
+        <c:crossAx val="538789568"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2281,12 +2281,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="51888640"/>
-        <c:axId val="110948288"/>
+        <c:axId val="539106816"/>
+        <c:axId val="538791872"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="51888640"/>
+        <c:axId val="539106816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110948288"/>
+        <c:crossAx val="538791872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2303,7 +2303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110948288"/>
+        <c:axId val="538791872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51888640"/>
+        <c:crossAx val="539106816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2622,12 +2622,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="51890688"/>
-        <c:axId val="110950592"/>
+        <c:axId val="542511616"/>
+        <c:axId val="538794176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="51890688"/>
+        <c:axId val="542511616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,7 +2636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110950592"/>
+        <c:crossAx val="538794176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2644,7 +2644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110950592"/>
+        <c:axId val="538794176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.75000000000000022"/>
@@ -2674,7 +2674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51890688"/>
+        <c:crossAx val="542511616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -20885,9 +20885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21200,25 +21200,25 @@
         <v>138</v>
       </c>
       <c r="C10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
         <v>139</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>140</v>
-      </c>
-      <c r="E10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" t="s">
-        <v>142</v>
       </c>
       <c r="G10" t="s">
         <v>143</v>
       </c>
       <c r="H10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" t="s">
         <v>144</v>
-      </c>
-      <c r="I10" t="s">
-        <v>145</v>
       </c>
       <c r="J10" t="s">
         <v>146</v>
@@ -52610,11 +52610,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK268"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G87" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB99" sqref="AB99"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -71118,16 +71118,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="23.7109375" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Added full autonomy in graph
</commit_message>
<xml_diff>
--- a/PathPlanner/UserStudyData/DataMyAnalysis.xlsx
+++ b/PathPlanner/UserStudyData/DataMyAnalysis.xlsx
@@ -1939,12 +1939,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cone"/>
-        <c:axId val="114681856"/>
-        <c:axId val="113960640"/>
-        <c:axId val="131745664"/>
+        <c:axId val="128641024"/>
+        <c:axId val="114747072"/>
+        <c:axId val="128272256"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="114681856"/>
+        <c:axId val="128641024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +1997,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113960640"/>
+        <c:crossAx val="114747072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2005,7 +2005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113960640"/>
+        <c:axId val="114747072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2016,12 +2016,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114681856"/>
+        <c:crossAx val="128641024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="131745664"/>
+        <c:axId val="128272256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2066,7 +2066,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113960640"/>
+        <c:crossAx val="114747072"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2341,12 +2341,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="117118464"/>
-        <c:axId val="113962944"/>
+        <c:axId val="131405312"/>
+        <c:axId val="114749376"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="117118464"/>
+        <c:axId val="131405312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2355,7 +2355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113962944"/>
+        <c:crossAx val="114749376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2363,7 +2363,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113962944"/>
+        <c:axId val="114749376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2393,7 +2393,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117118464"/>
+        <c:crossAx val="131405312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2683,12 +2683,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="117119488"/>
-        <c:axId val="113965248"/>
+        <c:axId val="131406848"/>
+        <c:axId val="114751680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="117119488"/>
+        <c:axId val="131406848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,7 +2697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113965248"/>
+        <c:crossAx val="114751680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2705,7 +2705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113965248"/>
+        <c:axId val="114751680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.75000000000000022"/>
@@ -2736,7 +2736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117119488"/>
+        <c:crossAx val="131406848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18804,7 +18804,7 @@
   <dimension ref="B5:AC83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>